<commit_message>
feat(inventory): improve inventory management UI - Add sorting functionality to grid view - Fix filtering in grid view - Enhance bar chart labels visibility - Improve monthly consumption chart display
</commit_message>
<xml_diff>
--- a/frontend/public/templates/product-template.xlsx
+++ b/frontend/public/templates/product-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,8 +407,9 @@
     <col min="3" max="3" customWidth="1" width="15"/>
     <col min="4" max="4" customWidth="1" width="15"/>
     <col min="5" max="5" customWidth="1" width="15"/>
-    <col min="6" max="6" customWidth="1" width="10"/>
-    <col min="7" max="7" customWidth="1" width="20"/>
+    <col min="6" max="6" customWidth="1" width="15"/>
+    <col min="7" max="7" customWidth="1" width="10"/>
+    <col min="8" max="8" customWidth="1" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -419,18 +420,21 @@
         <v>OUR CODE</v>
       </c>
       <c r="C1" t="str">
+        <v>ALT CODE</v>
+      </c>
+      <c r="D1" t="str">
         <v>DESIGN CODE</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>SUPPLIER</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>CATEGORY</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>GSM</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>CATALOGS</v>
       </c>
     </row>
@@ -442,24 +446,53 @@
         <v>501</v>
       </c>
       <c r="C2" t="str">
+        <v>501W</v>
+      </c>
+      <c r="D2" t="str">
         <v>9054-A</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>MBEE</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>Wooden</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>60</v>
       </c>
-      <c r="G2" t="str">
-        <v>Liner,Artis</v>
+      <c r="H2" t="str">
+        <v>Woodrica</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW COROBA</v>
+      </c>
+      <c r="B3" t="str">
+        <v>501A</v>
+      </c>
+      <c r="C3" t="str">
+        <v>501W</v>
+      </c>
+      <c r="D3" t="str">
+        <v>9054-A</v>
+      </c>
+      <c r="E3" t="str">
+        <v>MBEE</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Wooden</v>
+      </c>
+      <c r="G3" t="str">
+        <v>60</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Artvio</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>